<commit_message>
Finalized versions of test plans (formatted) and complete assignment pdf.
</commit_message>
<xml_diff>
--- a/Test Plan/Test_Case_4.2.1_helloworld.xlsx
+++ b/Test Plan/Test_Case_4.2.1_helloworld.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home02\rwiseman\Desktop\ECE411\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -169,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,93 +192,44 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,7 +514,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F13" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,105 +529,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="3"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -691,90 +642,84 @@
       <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
@@ -786,6 +731,12 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>